<commit_message>
Updated Backlog For Final Sprint
</commit_message>
<xml_diff>
--- a/Sprints/Sprint 4 Backlog and Burndown Chart.xlsx
+++ b/Sprints/Sprint 4 Backlog and Burndown Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimberlymiller/Documents/Computer Science 232/Project03/Sprints/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2ACDD0D2-AEE8-C844-93D2-E3340F51B532}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D35D5535-238F-6D48-8892-E500B932B172}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,12 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>User Story #1</t>
-  </si>
-  <si>
-    <t>Task</t>
   </si>
   <si>
     <t>User Story #2</t>
@@ -196,6 +193,18 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Fix the NoUTurnRoute</t>
+  </si>
+  <si>
+    <t>Fix the OnlyRightTurnRoute</t>
+  </si>
+  <si>
+    <t>UML/Backlog</t>
+  </si>
+  <si>
+    <t>Change customer orders</t>
   </si>
 </sst>
 </file>
@@ -968,8 +977,8 @@
   <dimension ref="B1:AG129"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q27" sqref="Q27"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -993,7 +1002,7 @@
   <sheetData>
     <row r="1" spans="2:33" ht="50" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -1029,52 +1038,52 @@
     </row>
     <row r="2" spans="2:33" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
@@ -1131,16 +1140,16 @@
     </row>
     <row r="4" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="8">
         <v>9</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="F4" s="8">
         <v>8</v>
@@ -1185,16 +1194,16 @@
     </row>
     <row r="5" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="8">
         <v>5</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="8">
         <v>6</v>
@@ -1239,16 +1248,16 @@
     </row>
     <row r="6" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="8">
         <v>7</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="8">
         <v>9</v>
@@ -1293,7 +1302,7 @@
     </row>
     <row r="7" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1329,16 +1338,16 @@
     </row>
     <row r="8" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="8">
         <v>7</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="8">
         <v>8</v>
@@ -1383,16 +1392,16 @@
     </row>
     <row r="9" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="8">
         <v>7</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="8">
         <v>15</v>
@@ -1437,16 +1446,16 @@
     </row>
     <row r="10" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="8">
         <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="8">
         <v>20</v>
@@ -1491,13 +1500,13 @@
     </row>
     <row r="11" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="8">
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8">
@@ -1537,7 +1546,7 @@
     </row>
     <row r="12" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1573,16 +1582,16 @@
     </row>
     <row r="13" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="8">
         <v>5</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" s="8">
         <v>4</v>
@@ -1637,16 +1646,16 @@
     </row>
     <row r="14" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="8">
         <v>7</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="8">
         <v>20</v>
@@ -1701,16 +1710,16 @@
     </row>
     <row r="15" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="8">
         <v>5</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="8">
         <v>2</v>
@@ -1765,16 +1774,16 @@
     </row>
     <row r="16" spans="2:33" ht="28" x14ac:dyDescent="0.15">
       <c r="B16" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="8">
         <v>10</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" s="8">
         <v>15</v>
@@ -1829,16 +1838,16 @@
     </row>
     <row r="17" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="8">
         <v>2</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" s="8">
         <v>3</v>
@@ -1893,16 +1902,16 @@
     </row>
     <row r="18" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="8">
         <v>7</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="8">
         <v>5</v>
@@ -1957,16 +1966,16 @@
     </row>
     <row r="19" spans="2:33" ht="28" x14ac:dyDescent="0.15">
       <c r="B19" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="8">
         <v>2</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F19" s="8">
         <v>13</v>
@@ -2021,7 +2030,7 @@
     </row>
     <row r="20" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -2057,14 +2066,14 @@
     </row>
     <row r="21" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F21" s="8">
         <v>5</v>
@@ -2117,14 +2126,14 @@
     </row>
     <row r="22" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F22" s="8">
         <v>20</v>
@@ -2177,11 +2186,11 @@
     </row>
     <row r="23" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
@@ -2215,11 +2224,11 @@
     </row>
     <row r="24" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
@@ -2253,11 +2262,11 @@
     </row>
     <row r="25" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -2291,7 +2300,7 @@
     </row>
     <row r="26" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -2327,14 +2336,14 @@
     </row>
     <row r="27" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F27" s="8">
         <v>1</v>
@@ -2387,7 +2396,7 @@
     </row>
     <row r="28" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -2423,10 +2432,14 @@
     </row>
     <row r="29" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
+        <v>54</v>
+      </c>
+      <c r="C29" s="8">
+        <v>6</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
@@ -2459,10 +2472,12 @@
     </row>
     <row r="30" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="8" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
+      <c r="D30" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
@@ -2495,7 +2510,7 @@
     </row>
     <row r="31" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="8" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -2531,10 +2546,12 @@
     </row>
     <row r="32" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="8" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
+      <c r="D32" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
@@ -2567,7 +2584,7 @@
     </row>
     <row r="33" spans="2:33" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>

</xml_diff>